<commit_message>
Update dictionary excel files
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/abundance.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/abundance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{456D7B3B-5807-4042-89C6-14E8907E0C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A9AFC-8860-A04F-AEA8-6D05D0992C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -740,9 +740,6 @@
     <t>abundanceCode</t>
   </si>
   <si>
-    <t>abundance.xml</t>
-  </si>
-  <si>
     <t>DIGGS Abundance Code Definitions</t>
   </si>
   <si>
@@ -891,6 +888,9 @@
   </si>
   <si>
     <t>Wentworth Scale (modified by Folk, 1954, 1974)</t>
+  </si>
+  <si>
+    <t>abundance</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1124,17 +1124,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1145,21 +1136,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1191,15 +1171,27 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1211,24 +1203,35 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color auto="1"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1300,6 +1303,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1332,50 +1356,6 @@
       </font>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1390,53 +1370,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DictionaryName" displayName="DictionaryName" ref="A1:E3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DictionaryName" displayName="DictionaryName" ref="A1:E3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Start" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Dictionary ID" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DictionaryFile" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DictionaryName" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Start" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Dictionary ID" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DictionaryFile" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DictionaryName" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:H19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H19">
     <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="11">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2827,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D42" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D42" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D42" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
     <sortCondition ref="B1:B42"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="2">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1724,8 +1704,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1769,13 +1749,13 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1837,432 +1817,409 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>266</v>
+      <c r="B2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>257</v>
+      <c r="G2" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="str">
+      <c r="A3" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="B3" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="18"/>
+      <c r="G3" s="19" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="str">
+      <c r="A4" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2831,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>250</v>
+        <v>244</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>249</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="str">
+      <c r="A5" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2839,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>265</v>
+      <c r="B5" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>257</v>
+      <c r="G5" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="str">
+      <c r="A6" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="H6" s="18"/>
+      <c r="G6" s="19" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="str">
+      <c r="A7" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2841,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>267</v>
+      <c r="B7" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>266</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>257</v>
+      <c r="G7" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="str">
+      <c r="A8" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2828,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>247</v>
+      <c r="B8" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>246</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="str">
+      <c r="A9" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2838,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>264</v>
+      <c r="B9" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>263</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>257</v>
+      <c r="G9" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="str">
+      <c r="A10" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2829,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>248</v>
+      <c r="B10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="str">
+      <c r="A11" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="str">
+      <c r="A12" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2832,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>251</v>
+      <c r="B12" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>250</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="str">
+      <c r="A13" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2837,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>263</v>
+      <c r="B13" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="27" t="s">
-        <v>268</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>257</v>
+      <c r="G13" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="str">
+      <c r="A14" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2833,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>252</v>
+      <c r="B14" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="18"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="str">
+      <c r="A15" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2836,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>262</v>
+      <c r="B15" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>261</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="27" t="s">
-        <v>283</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>257</v>
+      <c r="G15" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="str">
+      <c r="A16" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2834,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>253</v>
+      <c r="B16" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>252</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="18"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="str">
+      <c r="A17" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2830,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>249</v>
+      <c r="B17" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="str">
+      <c r="A18" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2835,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>254</v>
+      <c r="B18" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>253</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="18"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2827,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>246</v>
+      <c r="B19" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>245</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2249,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
@@ -2320,291 +2277,291 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="str">
+      <c r="A2" t="str">
         <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C4" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B3" s="25" t="s">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B4" s="28" t="s">
+      <c r="C5" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B5" s="28" t="s">
+      <c r="C20" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C21" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="C6" s="23" t="s">
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2612,203 +2569,203 @@
         <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B27" s="25" t="s">
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="str">
+        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C35" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="C29" s="23" t="s">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="str">
+        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="C32" s="23" t="s">
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="str">
+        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" t="str">
+        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="str">
+        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C33" s="3" t="s">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f>IF(ISNA(VLOOKUP(B41,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="C34" s="23" t="s">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="str">
+        <f>IF(ISNA(VLOOKUP(B42,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update codelist excel files
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/abundance.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/abundance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D0C660-40E1-244C-883B-985320CD871D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BCA379-CEF6-3743-9C0B-96A9DCF98228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20160" yWindow="8200" windowWidth="35840" windowHeight="19900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="284">
   <si>
     <t>Description</t>
   </si>
@@ -770,33 +770,6 @@
     <t>tertiary</t>
   </si>
   <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>Component descrbed  is present but estimated to be less than 5% by volume of the total feature described. It is used with "with" in a description such as "sand with trace clay"</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 5 to 10% by volume of the total feature described. It is used with "with" in a description such as "sand with few clay"</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 10 to 20% by volume of the total feature described. It is used with "with" in a description such as "sand with little clay"</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 20 to 35% by volume of the total feature described. It is used with "with" in a description such as "sand with some clay"</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises &gt;50% by volume of the total feature described. It defines the most dominant component (eg. Mostly sand with clay</t>
-  </si>
-  <si>
-    <t>Identifies the most common conponent observed.</t>
-  </si>
-  <si>
-    <t>Describes the second most common component observed</t>
-  </si>
-  <si>
-    <t>Describes the third most common component observed</t>
-  </si>
-  <si>
     <t>ASTM D2488</t>
   </si>
   <si>
@@ -818,24 +791,6 @@
     <t>dominant</t>
   </si>
   <si>
-    <t>Component descrbed  comprises &lt;5% by volume of the total feature described.</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 5 to 10% by volume of the total feature described.</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 10 to 20% by volume of the total feature described.</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 20 to 35% by volume of the total feature described.</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 35 to 50% by volume of the total feature described.</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises &gt;50% by volume of the total feature described.</t>
-  </si>
-  <si>
     <t>BS 5391</t>
   </si>
   <si>
@@ -854,24 +809,12 @@
     <t>common-BSCS</t>
   </si>
   <si>
-    <t>common-Folk</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 15 to 30% by volume of the total feature described.</t>
-  </si>
-  <si>
     <t>abundant-BSCS</t>
   </si>
   <si>
-    <t>abundant-Foik</t>
-  </si>
-  <si>
     <t>minor</t>
   </si>
   <si>
-    <t>Component descrbed  comprises 5 to 15% by volume of the total feature described.</t>
-  </si>
-  <si>
     <t>Wentworth (modified by Folk, 1954, 1974)</t>
   </si>
   <si>
@@ -887,10 +830,64 @@
     <t>quaternary</t>
   </si>
   <si>
-    <t>Describes the fourth most common component observed</t>
-  </si>
-  <si>
-    <t>Component descrbed  comprises 35 to 50% by volume of the total feature described. The term "and" is used to connect two components in a descriptive term with the dominant component listed last.</t>
+    <t>Identifies the most common conponent observed. Used in cases where percentages or percent estimates are not known or reported.</t>
+  </si>
+  <si>
+    <t>Describes the second most common component observed.  Used in cases where percentages or percent estimates are not known or reported.</t>
+  </si>
+  <si>
+    <t>Describes the third most common component observed.  Used in cases where percentages or percent estimates are not known or reported.</t>
+  </si>
+  <si>
+    <t>Describes the fourth most common component observed. Used in cases where percentages or percent estimates are not known or reported.</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>abundant</t>
+  </si>
+  <si>
+    <t>Component described  comprises 5 to 10% by volume of the total feature described. It is used with "with" in a description such as "sand with few clay"</t>
+  </si>
+  <si>
+    <t>Component described  comprises 10 to 20% by volume of the total feature described. It is used with "with" in a description such as "sand with little clay"</t>
+  </si>
+  <si>
+    <t>Component described  comprises &gt;50% by volume of the total feature described. It defines the most dominant component (eg. Mostly sand with clay</t>
+  </si>
+  <si>
+    <t>Component described  comprises 20 to 35% by volume of the total feature described. It is used with "with" in a description such as "sand with some clay"</t>
+  </si>
+  <si>
+    <t>Component described  is present but estimated to be less than 5% by volume of the total feature described. It is used with "with" in a description such as "sand with trace clay"</t>
+  </si>
+  <si>
+    <t>Component described  comprises 5 to 10% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 10 to 20% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 20 to 35% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 35 to 50% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises &lt;5% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises &gt;50% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 15 to 30% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 5 to 15% by volume of the total feature described.</t>
+  </si>
+  <si>
+    <t>Component described  comprises 30 to 50% by volume of the total feature described.</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1091,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1154,26 +1151,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1404,14 +1387,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:H20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:H19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H19">
-    <sortCondition ref="B1:B19"/>
+    <sortCondition ref="G1:G19"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="11">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2789,1,FALSE)),"Not used","")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2788,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="9"/>
@@ -1426,14 +1409,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D24" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:D24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
-    <sortCondition ref="C1:C23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D23" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:D23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D22">
+    <sortCondition ref="C1:C22"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="2">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="0"/>
@@ -1769,7 +1752,7 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>234</v>
@@ -1791,10 +1774,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1836,166 +1819,172 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2802,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2789,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B2" s="14" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2805,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B2790,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>275</v>
+      <c r="B3" s="14" t="s">
+        <v>238</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="E3" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2793,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="14" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2801,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B2791,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>271</v>
+      <c r="B5" s="25" t="s">
+        <v>239</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2804,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B2788,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>272</v>
+        <v>236</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>236</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="E6" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>279</v>
+        <v>244</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2803,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B2798,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" s="14" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>265</v>
+        <v>248</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>275</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2790,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B2799,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B8" s="14" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -2003,263 +1992,235 @@
         <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B2800,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>258</v>
+      <c r="B9" s="20" t="s">
+        <v>256</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>262</v>
+        <v>256</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>277</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2791,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B2801,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" s="14" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2806,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B2797,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" s="14" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="E11" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="G11" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2794,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B2802,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" s="14" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>280</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2799,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2804,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>257</v>
+      <c r="B13" s="17" t="s">
+        <v>269</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="E13" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2795,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2803,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2805,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="str">
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2794,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C16" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B2798,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2796,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>251</v>
+      <c r="D16" s="18" t="s">
+        <v>264</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2792,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2806,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>239</v>
+      <c r="B17" s="21" t="s">
+        <v>263</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E17" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2797,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2795,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>243</v>
+      <c r="B18" s="25" t="s">
+        <v>242</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>252</v>
+        <v>242</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>265</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2789,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>245</v>
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2796,1,FALSE)),"Not used","")</f>
+        <v>Not used</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>266</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2807,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="28"/>
+      <c r="G19" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -2275,7 +2236,7 @@
           <x14:formula1>
             <xm:f>Lists!$C$2:$C$178</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F20</xm:sqref>
+          <xm:sqref>F2:F19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2286,11 +2247,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2317,278 +2278,266 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B2" s="14" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B3" s="19" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B4" s="14" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B5" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B6" s="14" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B7" s="14" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B8" s="14" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B9" s="14" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B10" s="14" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B11" s="14" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B12" s="14" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B13" s="14" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B14" s="14" t="s">
         <v>241</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B15" s="14" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B16" s="14" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B17" s="14" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B18" s="14" t="s">
         <v>242</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B19" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B20" s="14" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B21" s="14" t="s">
         <v>243</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B22" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1812,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B23" s="14" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1813,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>282</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>